<commit_message>
a bunch of changes to OpenSRA.py to work with below ground infrastructure, scripts on below ground preprocessing logic, improved PC workflow
</commit_message>
<xml_diff>
--- a/examples/above_ground_shakemap/Results/results.xlsx
+++ b/examples/above_ground_shakemap/Results/results.xlsx
@@ -1665,16 +1665,16 @@
         <v>0</v>
       </c>
       <c r="DD2" t="n">
-        <v>9.775e-05</v>
+        <v>0.0002251</v>
       </c>
       <c r="DE2" t="n">
-        <v>0.004946</v>
+        <v>0.001169</v>
       </c>
       <c r="DF2" t="n">
-        <v>0.005958</v>
+        <v>0.001483</v>
       </c>
       <c r="DG2" t="n">
-        <v>0.003025</v>
+        <v>0.0006431</v>
       </c>
       <c r="DH2" t="n">
         <v>0</v>
@@ -1683,16 +1683,16 @@
         <v>0</v>
       </c>
       <c r="DJ2" t="n">
-        <v>0.0001506</v>
+        <v>0.0002136</v>
       </c>
       <c r="DK2" t="n">
-        <v>0.00351</v>
+        <v>0.001246</v>
       </c>
       <c r="DL2" t="n">
-        <v>0.0041</v>
+        <v>0.001471</v>
       </c>
       <c r="DM2" t="n">
-        <v>0.002008</v>
+        <v>0.0006898</v>
       </c>
       <c r="DN2" t="n">
         <v>0</v>
@@ -1701,16 +1701,16 @@
         <v>0</v>
       </c>
       <c r="DP2" t="n">
-        <v>0</v>
+        <v>0.0005961</v>
       </c>
       <c r="DQ2" t="n">
-        <v>0.009318999999999999</v>
+        <v>0.005942</v>
       </c>
       <c r="DR2" t="n">
-        <v>0.04027</v>
+        <v>0.009937</v>
       </c>
       <c r="DS2" t="n">
-        <v>0.01047</v>
+        <v>0.004479</v>
       </c>
       <c r="DT2" t="n">
         <v>0</v>
@@ -1719,16 +1719,16 @@
         <v>0</v>
       </c>
       <c r="DV2" t="n">
-        <v>0.0002813</v>
+        <v>0.0005432</v>
       </c>
       <c r="DW2" t="n">
-        <v>0.006808</v>
+        <v>0.004338</v>
       </c>
       <c r="DX2" t="n">
-        <v>0.008755000000000001</v>
+        <v>0.006215</v>
       </c>
       <c r="DY2" t="n">
-        <v>0.00488</v>
+        <v>0.003043</v>
       </c>
       <c r="DZ2" t="n">
         <v>0</v>
@@ -1737,16 +1737,16 @@
         <v>0</v>
       </c>
       <c r="EB2" t="n">
-        <v>0</v>
+        <v>0.0003913</v>
       </c>
       <c r="EC2" t="n">
-        <v>0.009082</v>
+        <v>0.002518</v>
       </c>
       <c r="ED2" t="n">
-        <v>0.01793</v>
+        <v>0.003136</v>
       </c>
       <c r="EE2" t="n">
-        <v>0.007742</v>
+        <v>0.001484</v>
       </c>
     </row>
     <row r="3">
@@ -2074,16 +2074,16 @@
         <v>0</v>
       </c>
       <c r="DD3" t="n">
-        <v>2.633e-05</v>
+        <v>7.014e-05</v>
       </c>
       <c r="DE3" t="n">
-        <v>0.0002428</v>
+        <v>0.0004082</v>
       </c>
       <c r="DF3" t="n">
-        <v>0.0004278</v>
+        <v>0.0006963</v>
       </c>
       <c r="DG3" t="n">
-        <v>0.0001547</v>
+        <v>0.0002639</v>
       </c>
       <c r="DH3" t="n">
         <v>0</v>
@@ -2092,16 +2092,16 @@
         <v>0</v>
       </c>
       <c r="DJ3" t="n">
-        <v>7.819e-05</v>
+        <v>0.0002273</v>
       </c>
       <c r="DK3" t="n">
-        <v>0.0007470000000000001</v>
+        <v>0.001183</v>
       </c>
       <c r="DL3" t="n">
-        <v>0.001152</v>
+        <v>0.001842</v>
       </c>
       <c r="DM3" t="n">
-        <v>0.0004877</v>
+        <v>0.0008363</v>
       </c>
       <c r="DN3" t="n">
         <v>0</v>
@@ -2110,16 +2110,16 @@
         <v>0</v>
       </c>
       <c r="DP3" t="n">
-        <v>1.791e-05</v>
+        <v>0.000723</v>
       </c>
       <c r="DQ3" t="n">
-        <v>0.00377</v>
+        <v>0.004759</v>
       </c>
       <c r="DR3" t="n">
-        <v>0.01642</v>
+        <v>0.02939</v>
       </c>
       <c r="DS3" t="n">
-        <v>0.00442</v>
+        <v>0.006789</v>
       </c>
       <c r="DT3" t="n">
         <v>0</v>
@@ -2128,16 +2128,16 @@
         <v>0</v>
       </c>
       <c r="DV3" t="n">
-        <v>0</v>
+        <v>0.0009963999999999999</v>
       </c>
       <c r="DW3" t="n">
-        <v>0.004493</v>
+        <v>0.005813</v>
       </c>
       <c r="DX3" t="n">
-        <v>0.03136</v>
+        <v>0.05211</v>
       </c>
       <c r="DY3" t="n">
-        <v>0.006518</v>
+        <v>0.009823</v>
       </c>
       <c r="DZ3" t="n">
         <v>0</v>
@@ -2146,16 +2146,16 @@
         <v>0</v>
       </c>
       <c r="EB3" t="n">
-        <v>9.432e-05</v>
+        <v>0.0001699</v>
       </c>
       <c r="EC3" t="n">
-        <v>0.0007703</v>
+        <v>0.0009661</v>
       </c>
       <c r="ED3" t="n">
-        <v>0.001275</v>
+        <v>0.001679</v>
       </c>
       <c r="EE3" t="n">
-        <v>0.0005096</v>
+        <v>0.0006628</v>
       </c>
     </row>
   </sheetData>
@@ -3174,16 +3174,16 @@
         <v>0</v>
       </c>
       <c r="DD2" t="n">
-        <v>0.001154</v>
+        <v>7.873e-05</v>
       </c>
       <c r="DE2" t="n">
-        <v>0.007621</v>
+        <v>0.002901</v>
       </c>
       <c r="DF2" t="n">
-        <v>0.009605000000000001</v>
+        <v>0.003468</v>
       </c>
       <c r="DG2" t="n">
-        <v>0.006337</v>
+        <v>0.001687</v>
       </c>
       <c r="DH2" t="n">
         <v>0</v>
@@ -3192,16 +3192,16 @@
         <v>0</v>
       </c>
       <c r="DJ2" t="n">
-        <v>0.0009805</v>
+        <v>0</v>
       </c>
       <c r="DK2" t="n">
-        <v>0.005723</v>
+        <v>0.002617</v>
       </c>
       <c r="DL2" t="n">
-        <v>0.00671</v>
+        <v>0.003009</v>
       </c>
       <c r="DM2" t="n">
-        <v>0.004162</v>
+        <v>0.001477</v>
       </c>
       <c r="DN2" t="n">
         <v>0</v>
@@ -3210,16 +3210,16 @@
         <v>0</v>
       </c>
       <c r="DP2" t="n">
-        <v>0.0007844</v>
+        <v>0.0001019</v>
       </c>
       <c r="DQ2" t="n">
-        <v>0.009771</v>
+        <v>0.007505</v>
       </c>
       <c r="DR2" t="n">
-        <v>0.07091</v>
+        <v>0.01052</v>
       </c>
       <c r="DS2" t="n">
-        <v>0.0173</v>
+        <v>0.006297</v>
       </c>
       <c r="DT2" t="n">
         <v>0</v>
@@ -3228,16 +3228,16 @@
         <v>0</v>
       </c>
       <c r="DV2" t="n">
-        <v>0.001053</v>
+        <v>0.0002161</v>
       </c>
       <c r="DW2" t="n">
-        <v>0.008286999999999999</v>
+        <v>0.006427</v>
       </c>
       <c r="DX2" t="n">
-        <v>0.02271</v>
+        <v>0.008392</v>
       </c>
       <c r="DY2" t="n">
-        <v>0.009258000000000001</v>
+        <v>0.004939</v>
       </c>
       <c r="DZ2" t="n">
         <v>0</v>
@@ -3246,16 +3246,16 @@
         <v>0</v>
       </c>
       <c r="EB2" t="n">
-        <v>0.001069</v>
+        <v>4.101e-05</v>
       </c>
       <c r="EC2" t="n">
-        <v>0.009853000000000001</v>
+        <v>0.004813</v>
       </c>
       <c r="ED2" t="n">
-        <v>0.0427</v>
+        <v>0.005891</v>
       </c>
       <c r="EE2" t="n">
-        <v>0.01336</v>
+        <v>0.00305</v>
       </c>
     </row>
     <row r="3">
@@ -3583,16 +3583,16 @@
         <v>0</v>
       </c>
       <c r="DD3" t="n">
-        <v>0.0001702</v>
+        <v>0.0001943</v>
       </c>
       <c r="DE3" t="n">
-        <v>0.001324</v>
+        <v>0.001957</v>
       </c>
       <c r="DF3" t="n">
-        <v>0.002504</v>
+        <v>0.003525</v>
       </c>
       <c r="DG3" t="n">
-        <v>0.001012</v>
+        <v>0.001291</v>
       </c>
       <c r="DH3" t="n">
         <v>0</v>
@@ -3601,17 +3601,17 @@
         <v>0</v>
       </c>
       <c r="DJ3" t="n">
-        <v>0.0001984</v>
+        <v>0.0002148</v>
       </c>
       <c r="DK3" t="n">
+        <v>0.003115</v>
+      </c>
+      <c r="DL3" t="n">
+        <v>0.005161</v>
+      </c>
+      <c r="DM3" t="n">
         <v>0.002257</v>
       </c>
-      <c r="DL3" t="n">
-        <v>0.003671</v>
-      </c>
-      <c r="DM3" t="n">
-        <v>0.001826</v>
-      </c>
       <c r="DN3" t="n">
         <v>0</v>
       </c>
@@ -3619,16 +3619,16 @@
         <v>0</v>
       </c>
       <c r="DP3" t="n">
-        <v>0.00135</v>
+        <v>0.000681</v>
       </c>
       <c r="DQ3" t="n">
-        <v>0.00613</v>
+        <v>0.007752</v>
       </c>
       <c r="DR3" t="n">
-        <v>0.06555</v>
+        <v>0.08286</v>
       </c>
       <c r="DS3" t="n">
-        <v>0.01204</v>
+        <v>0.01372</v>
       </c>
       <c r="DT3" t="n">
         <v>0</v>
@@ -3637,16 +3637,16 @@
         <v>0</v>
       </c>
       <c r="DV3" t="n">
-        <v>0.001413</v>
+        <v>0.0005789</v>
       </c>
       <c r="DW3" t="n">
-        <v>0.01981</v>
+        <v>0.02644</v>
       </c>
       <c r="DX3" t="n">
-        <v>0.1136</v>
+        <v>0.1395</v>
       </c>
       <c r="DY3" t="n">
-        <v>0.01999</v>
+        <v>0.02314</v>
       </c>
       <c r="DZ3" t="n">
         <v>0</v>
@@ -3655,16 +3655,16 @@
         <v>0</v>
       </c>
       <c r="EB3" t="n">
-        <v>0.0002798</v>
+        <v>0.0001511</v>
       </c>
       <c r="EC3" t="n">
-        <v>0.002609</v>
+        <v>0.002988</v>
       </c>
       <c r="ED3" t="n">
-        <v>0.004609</v>
+        <v>0.005618</v>
       </c>
       <c r="EE3" t="n">
-        <v>0.002206</v>
+        <v>0.002287</v>
       </c>
     </row>
   </sheetData>
@@ -3744,19 +3744,19 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.04953</v>
+        <v>0.04024</v>
       </c>
       <c r="F2" t="n">
-        <v>0.2866</v>
+        <v>0.2583</v>
       </c>
       <c r="G2" t="n">
-        <v>0.633</v>
+        <v>0.6158</v>
       </c>
       <c r="H2" t="n">
-        <v>0.8794</v>
+        <v>0.8424</v>
       </c>
       <c r="I2" t="n">
-        <v>0.3366</v>
+        <v>0.3207</v>
       </c>
     </row>
     <row r="3">
@@ -3775,19 +3775,19 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1229</v>
+        <v>0.1027</v>
       </c>
       <c r="F3" t="n">
-        <v>0.57</v>
+        <v>0.5762</v>
       </c>
       <c r="G3" t="n">
-        <v>0.9774</v>
+        <v>0.9725</v>
       </c>
       <c r="H3" t="n">
         <v>1</v>
       </c>
       <c r="I3" t="n">
-        <v>0.5506</v>
+        <v>0.543</v>
       </c>
     </row>
   </sheetData>
@@ -3910,16 +3910,16 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>9.775e-05</v>
+        <v>0.0002136</v>
       </c>
       <c r="G2" t="n">
-        <v>0.004946</v>
+        <v>0.001246</v>
       </c>
       <c r="H2" t="n">
-        <v>0.005958</v>
+        <v>0.001471</v>
       </c>
       <c r="I2" t="n">
-        <v>0.003025</v>
+        <v>0.0006898</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -3933,16 +3933,16 @@
         <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
+        <v>0.0005961</v>
       </c>
       <c r="N2" t="n">
-        <v>0.009318999999999999</v>
+        <v>0.005942</v>
       </c>
       <c r="O2" t="n">
-        <v>0.04027</v>
+        <v>0.009937</v>
       </c>
       <c r="P2" t="n">
-        <v>0.01047</v>
+        <v>0.004479</v>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
@@ -3969,16 +3969,16 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>7.819e-05</v>
+        <v>0.0002273</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0007470000000000001</v>
+        <v>0.001183</v>
       </c>
       <c r="H3" t="n">
-        <v>0.001152</v>
+        <v>0.001842</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0004877</v>
+        <v>0.0008363</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -3992,16 +3992,16 @@
         <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>0.0009963999999999999</v>
       </c>
       <c r="N3" t="n">
-        <v>0.004493</v>
+        <v>0.005813</v>
       </c>
       <c r="O3" t="n">
-        <v>0.03136</v>
+        <v>0.05211</v>
       </c>
       <c r="P3" t="n">
-        <v>0.006518</v>
+        <v>0.009823</v>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
@@ -4129,16 +4129,16 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.001154</v>
+        <v>7.873e-05</v>
       </c>
       <c r="G2" t="n">
-        <v>0.007621</v>
+        <v>0.002901</v>
       </c>
       <c r="H2" t="n">
-        <v>0.009605000000000001</v>
+        <v>0.003468</v>
       </c>
       <c r="I2" t="n">
-        <v>0.006337</v>
+        <v>0.001687</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -4152,16 +4152,16 @@
         <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0007844</v>
+        <v>0.0001019</v>
       </c>
       <c r="N2" t="n">
-        <v>0.009771</v>
+        <v>0.007505</v>
       </c>
       <c r="O2" t="n">
-        <v>0.07091</v>
+        <v>0.01052</v>
       </c>
       <c r="P2" t="n">
-        <v>0.0173</v>
+        <v>0.006297</v>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
@@ -4188,17 +4188,17 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0001984</v>
+        <v>0.0002148</v>
       </c>
       <c r="G3" t="n">
+        <v>0.003115</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.005161</v>
+      </c>
+      <c r="I3" t="n">
         <v>0.002257</v>
       </c>
-      <c r="H3" t="n">
-        <v>0.003671</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.001826</v>
-      </c>
       <c r="J3" t="inlineStr">
         <is>
           <t>jointA</t>
@@ -4211,16 +4211,16 @@
         <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>0.001413</v>
+        <v>0.0005789</v>
       </c>
       <c r="N3" t="n">
-        <v>0.01981</v>
+        <v>0.02644</v>
       </c>
       <c r="O3" t="n">
-        <v>0.1136</v>
+        <v>0.1395</v>
       </c>
       <c r="P3" t="n">
-        <v>0.01999</v>
+        <v>0.02314</v>
       </c>
       <c r="Q3" t="inlineStr">
         <is>

</xml_diff>